<commit_message>
added labs and update schedule information
</commit_message>
<xml_diff>
--- a/Recaps/HS2015_INTRO_Schedule.xlsx
+++ b/Recaps/HS2015_INTRO_Schedule.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="15330" windowHeight="6870" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="105" windowWidth="15330" windowHeight="6870"/>
   </bookViews>
   <sheets>
     <sheet name="Schedule" sheetId="1" r:id="rId1"/>
@@ -735,7 +735,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
@@ -1370,7 +1370,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:B27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added recap registration slots
</commit_message>
<xml_diff>
--- a/Recaps/HS2015_INTRO_Schedule.xlsx
+++ b/Recaps/HS2015_INTRO_Schedule.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="15330" windowHeight="6870" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="105" windowWidth="15330" windowHeight="6870"/>
   </bookViews>
   <sheets>
     <sheet name="Schedule" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="150">
   <si>
     <t>Week</t>
   </si>
@@ -283,9 +283,6 @@
     <t>Lindinger Kim</t>
   </si>
   <si>
-    <t>Mazlagic Ervin</t>
-  </si>
-  <si>
     <t>Moser Lucas</t>
   </si>
   <si>
@@ -404,6 +401,75 @@
   </si>
   <si>
     <t>05 42</t>
+  </si>
+  <si>
+    <t>L1</t>
+  </si>
+  <si>
+    <t>L2</t>
+  </si>
+  <si>
+    <t>L3</t>
+  </si>
+  <si>
+    <t>L4</t>
+  </si>
+  <si>
+    <t>L5</t>
+  </si>
+  <si>
+    <t>L6</t>
+  </si>
+  <si>
+    <t>18.9</t>
+  </si>
+  <si>
+    <t>Silvio Emmenegger</t>
+  </si>
+  <si>
+    <t>Pascal Häfliger</t>
+  </si>
+  <si>
+    <t>Roger Waltenspühl</t>
+  </si>
+  <si>
+    <t>Daniel Stadelmann</t>
+  </si>
+  <si>
+    <t>Cornel Emmenegger</t>
+  </si>
+  <si>
+    <t>Mario Fischer</t>
+  </si>
+  <si>
+    <t>Yves Studer</t>
+  </si>
+  <si>
+    <t>Bettina Wyss</t>
+  </si>
+  <si>
+    <t>Marcel Erismann</t>
+  </si>
+  <si>
+    <t>Michèle Rey</t>
+  </si>
+  <si>
+    <t>Jon Buchli</t>
+  </si>
+  <si>
+    <t>Marco Burgener, Simon Bucher</t>
+  </si>
+  <si>
+    <t>Cyrill Knüsel</t>
+  </si>
+  <si>
+    <t>Manuel Cattani</t>
+  </si>
+  <si>
+    <t>Kim Lindinger</t>
+  </si>
+  <si>
+    <t>David Niederberger</t>
   </si>
 </sst>
 </file>
@@ -435,7 +501,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -469,6 +535,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -537,7 +609,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -606,6 +678,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -903,8 +978,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -912,7 +987,8 @@
     <col min="1" max="1" width="4.140625" style="7" customWidth="1"/>
     <col min="2" max="2" width="11.5703125" customWidth="1"/>
     <col min="3" max="3" width="28" customWidth="1"/>
-    <col min="4" max="4" width="41.7109375" customWidth="1"/>
+    <col min="4" max="4" width="20" customWidth="1"/>
+    <col min="5" max="5" width="29" customWidth="1"/>
     <col min="6" max="6" width="27.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1010,7 +1086,10 @@
         <v>49</v>
       </c>
       <c r="D8" s="18" t="s">
-        <v>52</v>
+        <v>133</v>
+      </c>
+      <c r="E8" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -1020,6 +1099,9 @@
         <v>48</v>
       </c>
       <c r="D9" s="3"/>
+      <c r="E9" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="12">
@@ -1072,6 +1154,9 @@
       <c r="D14" s="18" t="s">
         <v>53</v>
       </c>
+      <c r="E14" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="8"/>
@@ -1080,6 +1165,9 @@
         <v>11</v>
       </c>
       <c r="D15" s="4"/>
+      <c r="E15" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="8"/>
@@ -1093,16 +1181,22 @@
       <c r="D16" s="18" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="17" spans="1:4">
+      <c r="E16" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17" s="8"/>
       <c r="B17" s="9"/>
       <c r="C17" s="10" t="s">
         <v>47</v>
       </c>
       <c r="D17" s="4"/>
-    </row>
-    <row r="18" spans="1:4" ht="13.5" customHeight="1">
+      <c r="E17" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="13.5" customHeight="1">
       <c r="A18" s="12">
         <v>5</v>
       </c>
@@ -1116,16 +1210,22 @@
       <c r="D18" s="18" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="19" spans="1:4">
+      <c r="E18" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
       <c r="A19" s="12"/>
       <c r="B19" s="14"/>
       <c r="C19" s="14" t="s">
         <v>46</v>
       </c>
       <c r="D19" s="4"/>
-    </row>
-    <row r="20" spans="1:4">
+      <c r="E19" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
       <c r="A20" s="12"/>
       <c r="B20" s="13">
         <f>B18+1</f>
@@ -1138,7 +1238,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:5">
       <c r="A21" s="12"/>
       <c r="B21" s="13"/>
       <c r="C21" s="16" t="s">
@@ -1146,7 +1246,7 @@
       </c>
       <c r="D21" s="6"/>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:5">
       <c r="A22" s="8">
         <v>6</v>
       </c>
@@ -1160,16 +1260,22 @@
       <c r="D22" s="18" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="23" spans="1:4">
+      <c r="E22" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
       <c r="A23" s="8"/>
       <c r="B23" s="9"/>
       <c r="C23" s="10" t="s">
         <v>12</v>
       </c>
       <c r="D23" s="4"/>
-    </row>
-    <row r="24" spans="1:4">
+      <c r="E23" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
       <c r="A24" s="8"/>
       <c r="B24" s="9">
         <f>B22+1</f>
@@ -1182,7 +1288,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:5">
       <c r="A25" s="8"/>
       <c r="B25" s="9"/>
       <c r="C25" s="10" t="s">
@@ -1190,7 +1296,7 @@
       </c>
       <c r="D25" s="3"/>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:5">
       <c r="A26" s="12">
         <v>7</v>
       </c>
@@ -1205,7 +1311,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:5">
       <c r="A27" s="12"/>
       <c r="B27" s="13"/>
       <c r="C27" s="14" t="s">
@@ -1213,7 +1319,7 @@
       </c>
       <c r="D27" s="3"/>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:5">
       <c r="A28" s="12"/>
       <c r="B28" s="13">
         <f>B26+1</f>
@@ -1225,16 +1331,22 @@
       <c r="D28" s="18" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="29" spans="1:4">
+      <c r="E28" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
       <c r="A29" s="12"/>
       <c r="B29" s="15"/>
       <c r="C29" s="14" t="s">
         <v>17</v>
       </c>
       <c r="D29" s="3"/>
-    </row>
-    <row r="30" spans="1:4">
+      <c r="E29" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
       <c r="A30" s="8">
         <v>8</v>
       </c>
@@ -1249,7 +1361,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:5">
       <c r="A31" s="8"/>
       <c r="B31" s="9"/>
       <c r="C31" s="10" t="s">
@@ -1257,7 +1369,7 @@
       </c>
       <c r="D31" s="3"/>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:5">
       <c r="A32" s="8"/>
       <c r="B32" s="9">
         <f>B30+1</f>
@@ -1269,16 +1381,22 @@
       <c r="D32" s="18" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="33" spans="1:4">
+      <c r="E32" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
       <c r="A33" s="8"/>
       <c r="B33" s="9"/>
       <c r="C33" s="10" t="s">
         <v>36</v>
       </c>
       <c r="D33" s="3"/>
-    </row>
-    <row r="34" spans="1:4">
+      <c r="E33" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
       <c r="A34" s="12">
         <v>9</v>
       </c>
@@ -1293,7 +1411,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:5">
       <c r="A35" s="12"/>
       <c r="B35" s="13"/>
       <c r="C35" s="14" t="s">
@@ -1301,7 +1419,7 @@
       </c>
       <c r="D35" s="3"/>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:5">
       <c r="A36" s="12"/>
       <c r="B36" s="13">
         <f>B34+1</f>
@@ -1314,13 +1432,13 @@
         <v>62</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:5">
       <c r="A37" s="12"/>
       <c r="B37" s="13"/>
       <c r="C37" s="15"/>
       <c r="D37" s="4"/>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:5">
       <c r="A38" s="8">
         <v>10</v>
       </c>
@@ -1335,7 +1453,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:5">
       <c r="A39" s="8"/>
       <c r="B39" s="9"/>
       <c r="C39" s="10" t="s">
@@ -1343,7 +1461,7 @@
       </c>
       <c r="D39" s="3"/>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:5">
       <c r="A40" s="8"/>
       <c r="B40" s="9">
         <f>B38+1</f>
@@ -1355,14 +1473,20 @@
       <c r="D40" s="18" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="41" spans="1:4">
+      <c r="E40" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
       <c r="A41" s="8"/>
       <c r="B41" s="9"/>
       <c r="C41" s="11"/>
       <c r="D41" s="3"/>
-    </row>
-    <row r="42" spans="1:4">
+      <c r="E41" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
       <c r="A42" s="12">
         <v>11</v>
       </c>
@@ -1377,13 +1501,13 @@
         <v>65</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:5">
       <c r="A43" s="12"/>
       <c r="B43" s="13"/>
       <c r="C43" s="14"/>
       <c r="D43" s="3"/>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:5">
       <c r="A44" s="12"/>
       <c r="B44" s="13">
         <f>B42+1</f>
@@ -1396,7 +1520,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
+    <row r="45" spans="1:5">
       <c r="A45" s="12"/>
       <c r="B45" s="13"/>
       <c r="C45" s="15" t="s">
@@ -1404,7 +1528,7 @@
       </c>
       <c r="D45" s="3"/>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" spans="1:5">
       <c r="A46" s="8">
         <v>12</v>
       </c>
@@ -1419,13 +1543,13 @@
         <v>67</v>
       </c>
     </row>
-    <row r="47" spans="1:4">
+    <row r="47" spans="1:5">
       <c r="A47" s="8"/>
       <c r="B47" s="9"/>
       <c r="C47" s="11"/>
       <c r="D47" s="3"/>
     </row>
-    <row r="48" spans="1:4">
+    <row r="48" spans="1:5">
       <c r="A48" s="8"/>
       <c r="B48" s="9">
         <f>B46+1</f>
@@ -1536,10 +1660,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K30"/>
+  <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1552,72 +1676,72 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B1" s="23"/>
       <c r="C1" s="23"/>
       <c r="D1" s="21">
-        <f>SUM(D3:D30)</f>
+        <f>SUM(D3:D29)</f>
+        <v>18</v>
+      </c>
+      <c r="E1" s="21">
+        <f>SUM(E3:E29)</f>
         <v>17</v>
       </c>
-      <c r="E1" s="21">
-        <f t="shared" ref="E1:J1" si="0">SUM(E3:E30)</f>
-        <v>16</v>
-      </c>
       <c r="F1" s="21">
-        <f t="shared" si="0"/>
-        <v>10</v>
+        <f>SUM(F3:F29)</f>
+        <v>11</v>
       </c>
       <c r="G1" s="21">
-        <f t="shared" si="0"/>
+        <f>SUM(G3:G29)</f>
         <v>17</v>
       </c>
       <c r="H1" s="21">
-        <f t="shared" si="0"/>
+        <f>SUM(H3:H29)</f>
         <v>15</v>
       </c>
       <c r="I1" s="21">
-        <f t="shared" si="0"/>
+        <f>SUM(I3:I29)</f>
         <v>3</v>
       </c>
       <c r="J1" s="21">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f>SUM(J3:J29)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B2" s="24" t="s">
+        <v>96</v>
+      </c>
+      <c r="C2" s="24" t="s">
+        <v>118</v>
+      </c>
+      <c r="D2" s="22" t="s">
+        <v>95</v>
+      </c>
+      <c r="E2" s="22" t="s">
         <v>97</v>
       </c>
-      <c r="C2" s="24" t="s">
-        <v>119</v>
-      </c>
-      <c r="D2" s="22" t="s">
-        <v>96</v>
-      </c>
-      <c r="E2" s="22" t="s">
+      <c r="F2" s="22" t="s">
         <v>98</v>
       </c>
-      <c r="F2" s="22" t="s">
+      <c r="G2" s="22" t="s">
         <v>99</v>
       </c>
-      <c r="G2" s="22" t="s">
+      <c r="H2" s="22" t="s">
+        <v>102</v>
+      </c>
+      <c r="I2" s="22" t="s">
         <v>100</v>
       </c>
-      <c r="H2" s="22" t="s">
+      <c r="J2" s="22" t="s">
+        <v>101</v>
+      </c>
+      <c r="K2" s="1" t="s">
         <v>103</v>
-      </c>
-      <c r="I2" s="22" t="s">
-        <v>101</v>
-      </c>
-      <c r="J2" s="22" t="s">
-        <v>102</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -1625,10 +1749,10 @@
         <v>83</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C3" s="27" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D3" s="21">
         <v>1</v>
@@ -1651,10 +1775,10 @@
         <v>85</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D4" s="21">
         <v>1</v>
@@ -1677,9 +1801,11 @@
         <v>86</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>117</v>
-      </c>
-      <c r="C5" s="23"/>
+        <v>116</v>
+      </c>
+      <c r="C5" s="27" t="s">
+        <v>119</v>
+      </c>
       <c r="D5" s="21">
         <v>1</v>
       </c>
@@ -1698,12 +1824,14 @@
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="20" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>117</v>
-      </c>
-      <c r="C6" s="23"/>
+        <v>116</v>
+      </c>
+      <c r="C6" s="33" t="s">
+        <v>127</v>
+      </c>
       <c r="D6" s="21"/>
       <c r="E6" s="21"/>
       <c r="F6" s="21">
@@ -1714,7 +1842,7 @@
       <c r="I6" s="21"/>
       <c r="J6" s="21"/>
       <c r="K6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -1722,9 +1850,9 @@
         <v>78</v>
       </c>
       <c r="B7" s="23" t="s">
-        <v>116</v>
-      </c>
-      <c r="C7" s="23"/>
+        <v>115</v>
+      </c>
+      <c r="C7" s="33"/>
       <c r="D7" s="30"/>
       <c r="E7" s="30"/>
       <c r="F7" s="30"/>
@@ -1735,12 +1863,14 @@
     </row>
     <row r="8" spans="1:11">
       <c r="A8" s="20" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B8" s="23" t="s">
-        <v>116</v>
-      </c>
-      <c r="C8" s="23"/>
+        <v>115</v>
+      </c>
+      <c r="C8" s="27" t="s">
+        <v>119</v>
+      </c>
       <c r="D8" s="32">
         <v>1</v>
       </c>
@@ -1764,9 +1894,11 @@
         <v>75</v>
       </c>
       <c r="B9" s="31" t="s">
-        <v>116</v>
-      </c>
-      <c r="C9" s="23"/>
+        <v>115</v>
+      </c>
+      <c r="C9" s="33" t="s">
+        <v>128</v>
+      </c>
       <c r="D9" s="21"/>
       <c r="E9" s="21"/>
       <c r="F9" s="21"/>
@@ -1780,10 +1912,10 @@
         <v>77</v>
       </c>
       <c r="B10" s="26" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C10" s="27" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D10" s="21">
         <v>1</v>
@@ -1808,10 +1940,10 @@
         <v>80</v>
       </c>
       <c r="B11" s="26" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C11" s="27" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D11" s="21">
         <v>1</v>
@@ -1825,30 +1957,38 @@
     </row>
     <row r="12" spans="1:11">
       <c r="A12" s="20" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B12" s="23" t="s">
-        <v>127</v>
-      </c>
-      <c r="C12" s="23"/>
-      <c r="D12" s="32"/>
-      <c r="E12" s="32"/>
-      <c r="F12" s="32"/>
+        <v>126</v>
+      </c>
+      <c r="C12" s="27" t="s">
+        <v>119</v>
+      </c>
+      <c r="D12" s="32">
+        <v>1</v>
+      </c>
+      <c r="E12" s="32">
+        <v>1</v>
+      </c>
+      <c r="F12" s="32">
+        <v>1</v>
+      </c>
       <c r="G12" s="32"/>
       <c r="H12" s="32"/>
       <c r="I12" s="32"/>
-      <c r="J12" s="30">
-        <v>1</v>
-      </c>
+      <c r="J12" s="32"/>
     </row>
     <row r="13" spans="1:11">
       <c r="A13" s="20" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B13" s="23" t="s">
-        <v>127</v>
-      </c>
-      <c r="C13" s="23"/>
+        <v>126</v>
+      </c>
+      <c r="C13" s="33" t="s">
+        <v>129</v>
+      </c>
       <c r="D13" s="32"/>
       <c r="E13" s="32"/>
       <c r="F13" s="32"/>
@@ -1866,10 +2006,10 @@
         <v>74</v>
       </c>
       <c r="B14" s="23" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C14" s="27" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D14" s="21">
         <v>1</v>
@@ -1894,10 +2034,10 @@
         <v>84</v>
       </c>
       <c r="B15" s="23" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C15" s="27" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D15" s="21">
         <v>1</v>
@@ -1919,13 +2059,13 @@
     </row>
     <row r="16" spans="1:11">
       <c r="A16" s="20" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B16" s="23" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C16" s="27" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D16" s="21">
         <v>1</v>
@@ -1945,13 +2085,13 @@
     </row>
     <row r="17" spans="1:10">
       <c r="A17" s="20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B17" s="23" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C17" s="27" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D17" s="21">
         <v>1</v>
@@ -1971,13 +2111,13 @@
     </row>
     <row r="18" spans="1:10">
       <c r="A18" s="20" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B18" s="23" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C18" s="27" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D18" s="21">
         <v>1</v>
@@ -2002,10 +2142,10 @@
         <v>71</v>
       </c>
       <c r="B19" s="23" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C19" s="27" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D19" s="21">
         <v>1</v>
@@ -2030,9 +2170,11 @@
         <v>81</v>
       </c>
       <c r="B20" s="23" t="s">
-        <v>111</v>
-      </c>
-      <c r="C20" s="23"/>
+        <v>110</v>
+      </c>
+      <c r="C20" s="33" t="s">
+        <v>130</v>
+      </c>
       <c r="D20" s="21"/>
       <c r="E20" s="21"/>
       <c r="F20" s="21"/>
@@ -2045,12 +2187,12 @@
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="20" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B21" s="23" t="s">
-        <v>111</v>
-      </c>
-      <c r="C21" s="23"/>
+        <v>110</v>
+      </c>
+      <c r="C21" s="33"/>
       <c r="D21" s="21"/>
       <c r="E21" s="21"/>
       <c r="F21" s="21"/>
@@ -2066,10 +2208,10 @@
         <v>76</v>
       </c>
       <c r="B22" s="23" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C22" s="27" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D22" s="21">
         <v>1</v>
@@ -2092,10 +2234,10 @@
         <v>79</v>
       </c>
       <c r="B23" s="23" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C23" s="27" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D23" s="21">
         <v>1</v>
@@ -2118,9 +2260,11 @@
         <v>69</v>
       </c>
       <c r="B24" s="23" t="s">
-        <v>109</v>
-      </c>
-      <c r="C24" s="23"/>
+        <v>108</v>
+      </c>
+      <c r="C24" s="33" t="s">
+        <v>131</v>
+      </c>
       <c r="D24" s="21"/>
       <c r="E24" s="21"/>
       <c r="F24" s="21"/>
@@ -2133,12 +2277,14 @@
     </row>
     <row r="25" spans="1:10">
       <c r="A25" s="20" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B25" s="23" t="s">
-        <v>109</v>
-      </c>
-      <c r="C25" s="23"/>
+        <v>108</v>
+      </c>
+      <c r="C25" s="27" t="s">
+        <v>119</v>
+      </c>
       <c r="D25" s="21">
         <v>1</v>
       </c>
@@ -2160,10 +2306,10 @@
         <v>70</v>
       </c>
       <c r="B26" s="23" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C26" s="27" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D26" s="21">
         <v>1</v>
@@ -2188,10 +2334,10 @@
         <v>72</v>
       </c>
       <c r="B27" s="23" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C27" s="27" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D27" s="21">
         <v>1</v>
@@ -2214,9 +2360,11 @@
         <v>73</v>
       </c>
       <c r="B28" s="23" t="s">
-        <v>107</v>
-      </c>
-      <c r="C28" s="23"/>
+        <v>106</v>
+      </c>
+      <c r="C28" s="33" t="s">
+        <v>132</v>
+      </c>
       <c r="D28" s="21"/>
       <c r="E28" s="21"/>
       <c r="F28" s="21"/>
@@ -2240,20 +2388,6 @@
       <c r="H29" s="21"/>
       <c r="I29" s="21"/>
       <c r="J29" s="21"/>
-    </row>
-    <row r="30" spans="1:10">
-      <c r="A30" s="28" t="s">
-        <v>87</v>
-      </c>
-      <c r="B30" s="29"/>
-      <c r="C30" s="29"/>
-      <c r="D30" s="21"/>
-      <c r="E30" s="21"/>
-      <c r="F30" s="21"/>
-      <c r="G30" s="21"/>
-      <c r="H30" s="21"/>
-      <c r="I30" s="21"/>
-      <c r="J30" s="21"/>
     </row>
   </sheetData>
   <autoFilter ref="A2:K2">
@@ -2285,7 +2419,7 @@
         <v>7</v>
       </c>
       <c r="B1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -2293,7 +2427,7 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -2301,7 +2435,7 @@
         <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -2309,7 +2443,7 @@
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -2317,7 +2451,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>

</xml_diff>